<commit_message>
Add plot validation, fix #427
</commit_message>
<xml_diff>
--- a/docs/tutorial/assets/T1/t1_framework_1.xlsx
+++ b/docs/tutorial/assets/T1/t1_framework_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\docs\tutorial\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh\projects\atomica\docs\tutorial\assets\T1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FB0067-EABA-47A8-8EB7-10F225AD6DDB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1162D6-F679-4ED0-AF07-2A77DF545222}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="420" windowWidth="21225" windowHeight="17085" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3435" yWindow="4740" windowWidth="28800" windowHeight="15435" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -21,15 +21,16 @@
     <sheet name="Characteristics" sheetId="4" r:id="rId6"/>
     <sheet name="Parameters" sheetId="6" r:id="rId7"/>
     <sheet name="Interactions" sheetId="5" r:id="rId8"/>
-    <sheet name="Cascades" sheetId="7" r:id="rId9"/>
-    <sheet name="Plots" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2765,173 +2766,8 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Romesh</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B935E62C-0938-0C4C-AF10-F1E1867CC167}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Specify the name of your cascade in this cell. In the cells below, specify the names of your cascade's stages
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-cascades</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{E94A098B-5A50-AA4C-99A6-0D4002426718}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">In this column, specify which compartments and characteristics make up each cascade stage. You should specify them as a comma separated list of code names e.g., 'sus, inf, rec'
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-cascades</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{2EB6BD31-E926-014E-9F7A-805DBC8C7D8D}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The code name should be in lower case without spaces.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">For further instructions on how to fill this out, please see cascade.tools/ug-frw-plots
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{F09145A5-5E42-3A46-99A0-F87F2F2A0381}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">The display name will appear in plots and other outputs. It should be in sentence case.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>For further instructions on how to fill this out, please see cascade.tools/ug-frw-plots</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>Datasheet Code Name</t>
   </si>
@@ -2943,12 +2779,6 @@
   </si>
   <si>
     <t>Display Name</t>
-  </si>
-  <si>
-    <t>Compartment 1</t>
-  </si>
-  <si>
-    <t>Compartment 2</t>
   </si>
   <si>
     <t>Is Source</t>
@@ -2990,39 +2820,6 @@
     <t>Function</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Quantities</t>
-  </si>
-  <si>
-    <t>Aggregate pops</t>
-  </si>
-  <si>
-    <t>Plot Group</t>
-  </si>
-  <si>
-    <t>comp2</t>
-  </si>
-  <si>
-    <t>comp1</t>
-  </si>
-  <si>
-    <t>Constituents</t>
-  </si>
-  <si>
-    <t>series</t>
-  </si>
-  <si>
-    <t>alive</t>
-  </si>
-  <si>
-    <t>both</t>
-  </si>
-  <si>
-    <t>{'All':['comp1','comp2']}</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -3051,9 +2848,6 @@
   </si>
   <si>
     <t>This is a template cascade. For instructions on how to fill it out, please see: cascade.tools/user-guide</t>
-  </si>
-  <si>
-    <t>Cascade name</t>
   </si>
   <si>
     <t>Guidance</t>
@@ -3171,7 +2965,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3214,25 +3008,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -3729,108 +3504,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6A2575B-90FD-4432-ABB5-1D1C9A3EC31C}">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{B6FB0777-9CB4-4E7A-978E-F88EC2A52ADA}">
-      <formula1>"n,y"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3861,18 +3551,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3910,18 +3600,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3937,7 +3627,7 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -3964,42 +3654,42 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4009,44 +3699,44 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -5720,7 +5410,7 @@
         <v>birth</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:398" x14ac:dyDescent="0.25">
@@ -5729,10 +5419,10 @@
         <v>sus</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:398" x14ac:dyDescent="0.25">
@@ -5741,10 +5431,10 @@
         <v>inf</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:398" x14ac:dyDescent="0.25">
@@ -5753,7 +5443,7 @@
         <v>rec</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:398" x14ac:dyDescent="0.25">
@@ -8182,31 +7872,31 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -8309,74 +7999,74 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="L1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="K2" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L2" s="2"/>
       <c r="N2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -8386,68 +8076,68 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="K3" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="L3" s="2"/>
       <c r="N3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" t="s">
         <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="E6" s="2">
         <v>0.1</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -8544,13 +8234,13 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8579,38 +8269,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1EAFB5-C4B0-491C-B03B-D10386E1B6D4}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="55.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>